<commit_message>
Changes in Gensen Excel Process
</commit_message>
<xml_diff>
--- a/resources/assets/uploadandtemplates/templates/gensen_Payment.xlsx
+++ b/resources/assets/uploadandtemplates/templates/gensen_Payment.xlsx
@@ -29,7 +29,7 @@
       </rPr>
       <t>OB</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -45,7 +45,7 @@
       </rPr>
       <t>ather</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -61,7 +61,7 @@
       </rPr>
       <t>other</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -77,7 +77,7 @@
       </rPr>
       <t>erson</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -93,7 +93,7 @@
       </rPr>
       <t>ana</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -109,7 +109,7 @@
       </rPr>
       <t>ame</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -125,7 +125,7 @@
       </rPr>
       <t>ddress</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -141,7 +141,7 @@
       </rPr>
       <t>alary</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -157,7 +157,7 @@
       </rPr>
       <t>eduction</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <r>
@@ -173,23 +173,23 @@
       </rPr>
       <t>mp no</t>
     </r>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Kana Name</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Insurance</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>生年月日</t>
-    <phoneticPr fontId="3"/>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -203,13 +203,6 @@
       <name val="ＭＳ Ｐゴシック"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="MS UI Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -219,6 +212,13 @@
     <font>
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="MS UI Gothic"/>
       <family val="3"/>
       <charset val="128"/>
     </font>
@@ -266,7 +266,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="38" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="38" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -274,35 +274,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="distributed" vertical="center"/>
-    </xf>
-    <xf numFmtId="57" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="38" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="center"/>
+    </xf>
+    <xf numFmtId="57" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -614,7 +614,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="9"/>
+      <c r="A1" s="6"/>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="3" t="s">
@@ -626,9 +626,9 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="10" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -636,17 +636,17 @@
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:7" ht="37.5" customHeight="1">
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="13" spans="1:7">
       <c r="C13" s="1"/>
@@ -671,18 +671,18 @@
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="1"/>
     </row>
     <row r="18" spans="2:4">
@@ -697,16 +697,16 @@
       </c>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
     <mergeCell ref="C11:E11"/>
   </mergeCells>
-  <phoneticPr fontId="3"/>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>